<commit_message>
Rendre numero_article optionnel pour la création d\'article
Co-authored-by: Capy <capy@capy.ai>
</commit_message>
<xml_diff>
--- a/apps/web/public/templates/article_import_template.xlsx
+++ b/apps/web/public/templates/article_import_template.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,11 +437,6 @@
           <t>numero_fournisseur_unique</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>numero_article</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>